<commit_message>
enhanced URL combination validation
</commit_message>
<xml_diff>
--- a/combination.xlsx
+++ b/combination.xlsx
@@ -504,15 +504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -525,16 +516,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,13 +1014,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -1042,129 +1042,129 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
@@ -1175,33 +1175,33 @@
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="27"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="27"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="30"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="31"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
@@ -1269,15 +1269,15 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A30" s="32"/>
-      <c r="B30" s="33" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
@@ -1286,113 +1286,113 @@
     </row>
     <row r="32" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="33"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="33"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
@@ -1474,243 +1474,243 @@
       <c r="B59" s="17"/>
     </row>
     <row r="60" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="31" t="s">
         <v>48</v>
       </c>
       <c r="B60" s="17"/>
-      <c r="C60" s="35" t="s">
+      <c r="C60" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="18"/>
+      <c r="A61" s="32"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="35"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
     </row>
     <row r="62" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="18"/>
+      <c r="A62" s="32"/>
       <c r="B62" s="17"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="18"/>
+      <c r="A63" s="32"/>
       <c r="B63" s="17"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="18"/>
+      <c r="A64" s="32"/>
       <c r="B64" s="17"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="35"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" s="18"/>
+      <c r="A65" s="32"/>
       <c r="B65" s="17"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="35"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="18"/>
+      <c r="A66" s="32"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="35"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="35"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="18"/>
+      <c r="A67" s="32"/>
       <c r="B67" s="17"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="18"/>
+      <c r="A68" s="32"/>
       <c r="B68" s="17"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="35"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="18"/>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
+      <c r="A69" s="32"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="18"/>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="35"/>
+      <c r="A70" s="32"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="18"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
+      <c r="A71" s="32"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="31"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="18"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
+      <c r="A72" s="32"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="18"/>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
+      <c r="A73" s="32"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="31"/>
+      <c r="F73" s="31"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="18"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="35"/>
+      <c r="A74" s="32"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="18"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
+      <c r="A75" s="32"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="18"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="35"/>
+      <c r="A76" s="32"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="18"/>
-      <c r="C77" s="35"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="35"/>
+      <c r="A77" s="32"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="18"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="35"/>
+      <c r="A78" s="32"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A79" s="18"/>
-      <c r="C79" s="35"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="35"/>
+      <c r="A79" s="32"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A80" s="18"/>
-      <c r="C80" s="35"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="35"/>
-      <c r="F80" s="35"/>
+      <c r="A80" s="32"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="31"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="31"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81" s="18"/>
-      <c r="C81" s="35"/>
-      <c r="D81" s="35"/>
-      <c r="E81" s="35"/>
-      <c r="F81" s="35"/>
+      <c r="A81" s="32"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="31"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" s="18"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="35"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="35"/>
+      <c r="A82" s="32"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A83" s="18"/>
-      <c r="C83" s="35"/>
-      <c r="D83" s="35"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="35"/>
+      <c r="A83" s="32"/>
+      <c r="C83" s="31"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="31"/>
+      <c r="F83" s="31"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" s="18"/>
-      <c r="C84" s="35"/>
-      <c r="D84" s="35"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="35"/>
+      <c r="A84" s="32"/>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" s="18"/>
-      <c r="C85" s="35"/>
-      <c r="D85" s="35"/>
-      <c r="E85" s="35"/>
-      <c r="F85" s="35"/>
+      <c r="A85" s="32"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="18"/>
-      <c r="C86" s="35"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="35"/>
+      <c r="A86" s="32"/>
+      <c r="C86" s="31"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="31"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" s="18"/>
-      <c r="C87" s="35"/>
-      <c r="D87" s="35"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="35"/>
+      <c r="A87" s="32"/>
+      <c r="C87" s="31"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="31"/>
+      <c r="F87" s="31"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" s="18"/>
+      <c r="A88" s="32"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89" s="18"/>
+      <c r="A89" s="32"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90" s="18"/>
+      <c r="A90" s="32"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91" s="18"/>
+      <c r="A91" s="32"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" s="18"/>
+      <c r="A92" s="32"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A93" s="36"/>
+      <c r="A93" s="30"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A94" s="36"/>
+      <c r="A94" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B1:F1"/>
     <mergeCell ref="A60:A92"/>
     <mergeCell ref="C60:F87"/>
     <mergeCell ref="B32:O37"/>
     <mergeCell ref="C5:O11"/>
     <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
solved combination of non-required parameter
</commit_message>
<xml_diff>
--- a/combination.xlsx
+++ b/combination.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
   <si>
     <t>groupBy=FAC</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>customDate=2020/04/01-2020/05/19</t>
-  </si>
-  <si>
-    <t>customDate=2020-03-18 to 2020-05-23</t>
   </si>
   <si>
     <t>fabLocation=AMKORK4</t>
@@ -163,10 +160,6 @@
 http://total.itg.ti.com/ToTaL/?timestamp=1570+groupBy=SBE&amp;sbe=AFS 
 http://total.itg.ti.com/ToTaL/?timestamp=1570+groupBy=SBE&amp;sbe1=BMC 
 </t>
-  </si>
-  <si>
-    <t>*possible bang maulit sa URL ang PARAMETER
-http://total.itg.ti.com/ToTaL/?timestamp=1590126090970+fabLocation=AMKORK4&amp;fabLocation=AMKORK4</t>
   </si>
   <si>
     <t>groupBy=FAC
@@ -233,12 +226,77 @@
 device=$4771773G
 fablot=0000001</t>
   </si>
+  <si>
+    <t>filterFacility</t>
+  </si>
+  <si>
+    <t>filterTechnology</t>
+  </si>
+  <si>
+    <t>filterSBE</t>
+  </si>
+  <si>
+    <t>filterDevice</t>
+  </si>
+  <si>
+    <t>filterLot</t>
+  </si>
+  <si>
+    <t>local=dallas</t>
+  </si>
+  <si>
+    <t>local=local</t>
+  </si>
+  <si>
+    <t>tranDate=2020-03-18 to 2020-05-23</t>
+  </si>
+  <si>
+    <t>tranDate=L30D</t>
+  </si>
+  <si>
+    <t>tranDate=LM</t>
+  </si>
+  <si>
+    <t>tranDate=LQ</t>
+  </si>
+  <si>
+    <t>tranDate=MTD</t>
+  </si>
+  <si>
+    <t>tranDate=QTD</t>
+  </si>
+  <si>
+    <t>tranDate=YTD</t>
+  </si>
+  <si>
+    <t>columns=0,1,2</t>
+  </si>
+  <si>
+    <t>filterColumn</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Combination</t>
+  </si>
+  <si>
+    <t>1456*1919 = 2,794,064‬</t>
+  </si>
+  <si>
+    <t>Non required
+Parameter</t>
+  </si>
+  <si>
+    <t>Required &amp; non-required
+combination</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +331,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,8 +401,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -477,11 +549,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -517,6 +783,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -535,8 +803,58 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,26 +1322,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45:K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.54296875" customWidth="1"/>
-    <col min="3" max="4" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -1045,129 +1367,129 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
+      <c r="C5" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
@@ -1228,533 +1550,720 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="29"/>
-      <c r="B30" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
+      <c r="B30" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
-      <c r="B32" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="59"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="59"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="34"/>
+        <v>45</v>
+      </c>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="59"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="34"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="59"/>
+      <c r="N34" s="59"/>
+      <c r="O34" s="59"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="34"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="59"/>
+      <c r="K35" s="59"/>
+      <c r="L35" s="59"/>
+      <c r="M35" s="59"/>
+      <c r="N35" s="59"/>
+      <c r="O35" s="59"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="59"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="59"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="59"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="34"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+    </row>
+    <row r="38" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="I39" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J39" s="52"/>
+    </row>
+    <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B40" s="34"/>
+      <c r="I40" s="60"/>
+      <c r="J40" s="53" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
+      <c r="B41" s="34"/>
+      <c r="E41" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="40"/>
       <c r="G41" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="I41" s="54">
+        <v>1</v>
+      </c>
+      <c r="J41" s="53"/>
+    </row>
+    <row r="42" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E42" s="41"/>
+      <c r="F42" s="42"/>
       <c r="G42" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="I42" s="54">
+        <v>2</v>
+      </c>
+      <c r="J42" s="53"/>
+    </row>
+    <row r="43" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B43" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="52"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="42"/>
       <c r="G43" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="I43" s="54">
+        <v>3</v>
+      </c>
+      <c r="J43" s="53"/>
+    </row>
+    <row r="44" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" s="41"/>
+      <c r="F44" s="42"/>
       <c r="G44" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="I44" s="54">
+        <v>4</v>
+      </c>
+      <c r="J44" s="53"/>
+    </row>
+    <row r="45" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B45" s="54">
+        <v>1</v>
+      </c>
+      <c r="C45" s="53">
+        <v>16</v>
+      </c>
+      <c r="E45" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" s="42"/>
       <c r="G45" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="I45" s="54">
+        <v>5</v>
+      </c>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="9"/>
+      <c r="B46" s="54">
+        <v>2</v>
+      </c>
+      <c r="C46" s="53">
+        <v>104</v>
+      </c>
+      <c r="E46" s="41"/>
+      <c r="F46" s="42"/>
       <c r="G46" s="4" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I46" s="54">
+        <v>6</v>
+      </c>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
-        <v>40</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B47" s="54">
+        <v>3</v>
+      </c>
+      <c r="C47" s="53">
+        <v>350</v>
+      </c>
+      <c r="E47" s="41"/>
+      <c r="F47" s="42"/>
       <c r="G47" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I47" s="54">
+        <v>7</v>
+      </c>
+      <c r="J47" s="53"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="54">
+        <v>4</v>
+      </c>
+      <c r="C48" s="53">
+        <v>639</v>
+      </c>
+      <c r="E48" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F48" s="42"/>
+      <c r="G48" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I48" s="54">
+        <v>8</v>
+      </c>
+      <c r="J48" s="53"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" s="11"/>
+      <c r="B49" s="54">
+        <v>5</v>
+      </c>
+      <c r="C49" s="53">
+        <v>594</v>
+      </c>
+      <c r="E49" s="41"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49" s="54">
+        <v>9</v>
+      </c>
+      <c r="J49" s="53"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="54">
+        <v>6</v>
+      </c>
+      <c r="C50" s="55">
+        <v>216</v>
+      </c>
+      <c r="E50" s="41"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="I50" s="54">
+        <v>10</v>
+      </c>
+      <c r="J50" s="53"/>
+    </row>
+    <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="11"/>
+      <c r="B51" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="57">
+        <f>SUM(C45:C50)</f>
+        <v>1919</v>
+      </c>
+      <c r="E51" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="42"/>
+      <c r="G51" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="11"/>
-      <c r="G49" s="8" t="s">
+      <c r="I51" s="54">
+        <v>11</v>
+      </c>
+      <c r="J51" s="53"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="41"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
+      <c r="I52" s="54">
+        <v>12</v>
+      </c>
+      <c r="J52" s="53"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="50"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G50" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="11"/>
-      <c r="G51" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="10" t="s">
+      <c r="I53" s="54">
+        <v>13</v>
+      </c>
+      <c r="J53" s="53"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54" s="13"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="E54" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" s="42"/>
+      <c r="G54" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G52" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="12" t="s">
+      <c r="I54" s="54">
+        <v>14</v>
+      </c>
+      <c r="J54" s="53"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G53" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="13"/>
-      <c r="G54" s="12" t="s">
+      <c r="B55" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="50"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G56" s="37"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G57" s="37"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G58" s="37"/>
-    </row>
-    <row r="59" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I55" s="54">
+        <v>15</v>
+      </c>
+      <c r="J55" s="53"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" s="48"/>
+      <c r="G56" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="I56" s="54">
+        <v>16</v>
+      </c>
+      <c r="J56" s="53"/>
+    </row>
+    <row r="57" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E57" s="46"/>
+      <c r="G57" s="31"/>
+      <c r="I57" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="J57" s="57"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G58" s="31"/>
+    </row>
+    <row r="59" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="17"/>
-      <c r="G59" s="37"/>
-    </row>
-    <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="32" t="s">
-        <v>50</v>
+      <c r="G59" s="31"/>
+    </row>
+    <row r="60" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="34" t="s">
+        <v>48</v>
       </c>
       <c r="B60" s="17"/>
-      <c r="C60" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="38"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="33"/>
+      <c r="C60" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="32"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A61" s="35"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-    </row>
-    <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="33"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+    </row>
+    <row r="62" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="35"/>
       <c r="B62" s="17"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="33"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A63" s="35"/>
       <c r="B63" s="17"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="33"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A64" s="35"/>
       <c r="B64" s="17"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" s="33"/>
+      <c r="A65" s="35"/>
       <c r="B65" s="17"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="33"/>
+      <c r="A66" s="35"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="33"/>
+      <c r="A67" s="35"/>
       <c r="B67" s="17"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="34"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="33"/>
+      <c r="A68" s="35"/>
       <c r="B68" s="17"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="34"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="33"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
+      <c r="A69" s="35"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="33"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
+      <c r="A70" s="35"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="34"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="33"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="32"/>
+      <c r="A71" s="35"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="34"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="33"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
+      <c r="A72" s="35"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="33"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
+      <c r="A73" s="35"/>
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="34"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="33"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="32"/>
+      <c r="A74" s="35"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="33"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="32"/>
+      <c r="A75" s="35"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="34"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="33"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
+      <c r="A76" s="35"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="34"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="33"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="32"/>
+      <c r="A77" s="35"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="34"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="33"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="32"/>
+      <c r="A78" s="35"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="34"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A79" s="33"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="32"/>
+      <c r="A79" s="35"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="34"/>
+      <c r="F79" s="34"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A80" s="33"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="32"/>
+      <c r="A80" s="35"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81" s="33"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="32"/>
+      <c r="A81" s="35"/>
+      <c r="C81" s="34"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="34"/>
+      <c r="F81" s="34"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" s="33"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="32"/>
-      <c r="F82" s="32"/>
+      <c r="A82" s="35"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="34"/>
+      <c r="F82" s="34"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A83" s="33"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="32"/>
-      <c r="F83" s="32"/>
+      <c r="A83" s="35"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="34"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" s="33"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="32"/>
-      <c r="E84" s="32"/>
-      <c r="F84" s="32"/>
+      <c r="A84" s="35"/>
+      <c r="C84" s="34"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="34"/>
+      <c r="F84" s="34"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" s="33"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="32"/>
+      <c r="A85" s="35"/>
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="34"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="33"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="32"/>
+      <c r="A86" s="35"/>
+      <c r="C86" s="34"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="34"/>
+      <c r="F86" s="34"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" s="33"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="32"/>
+      <c r="A87" s="35"/>
+      <c r="C87" s="34"/>
+      <c r="D87" s="34"/>
+      <c r="E87" s="34"/>
+      <c r="F87" s="34"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" s="33"/>
+      <c r="A88" s="35"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89" s="33"/>
+      <c r="A89" s="35"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90" s="33"/>
+      <c r="A90" s="35"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91" s="33"/>
+      <c r="A91" s="35"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" s="33"/>
+      <c r="A92" s="35"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="30"/>
@@ -1763,13 +2272,23 @@
       <c r="A94" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="16">
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B53:C54"/>
+    <mergeCell ref="I39:I40"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A60:A92"/>
     <mergeCell ref="C60:F87"/>
-    <mergeCell ref="B32:O37"/>
     <mergeCell ref="C5:O11"/>
     <mergeCell ref="B30:E30"/>
+    <mergeCell ref="E41:F44"/>
+    <mergeCell ref="E45:F47"/>
+    <mergeCell ref="E48:F50"/>
+    <mergeCell ref="E51:F53"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B40:B41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>